<commit_message>
ExcelPriceReader implementation + test
</commit_message>
<xml_diff>
--- a/src/test/resources/excelPriceReader/testSupplier/pricetepark.xlsx
+++ b/src/test/resources/excelPriceReader/testSupplier/pricetepark.xlsx
@@ -133,10 +133,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -421,7 +423,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -474,7 +476,7 @@
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -491,7 +493,7 @@
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -508,7 +510,7 @@
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -517,5 +519,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>